<commit_message>
Added the drag model for high mach number
</commit_message>
<xml_diff>
--- a/code/var/1976_standard_ATM.xlsx
+++ b/code/var/1976_standard_ATM.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seb\Documents\Codes\LagTrack\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastien/Documents/Codes/LagTrack/code/var/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF76E4D-2B9D-B64A-A927-2EAC4D3F67AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14340" windowHeight="7515"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29300" windowHeight="25960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,14 +25,32 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -54,11 +73,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -338,16 +360,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="8.83203125" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -357,8 +382,16 @@
       <c r="C1" s="1">
         <v>1.8120600000000001E-5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="4">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>500</v>
       </c>
@@ -368,8 +401,16 @@
       <c r="C2" s="1">
         <v>1.79579E-5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="4">
+        <v>11.75</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1000</v>
       </c>
@@ -379,8 +420,16 @@
       <c r="C3" s="1">
         <v>1.77943E-5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="4">
+        <v>8.5</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1500</v>
       </c>
@@ -390,8 +439,16 @@
       <c r="C4" s="1">
         <v>1.7629799999999998E-5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="4">
+        <v>5.25</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2000</v>
       </c>
@@ -401,8 +458,16 @@
       <c r="C5" s="1">
         <v>1.7464499999999999E-5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2500</v>
       </c>
@@ -412,8 +477,16 @@
       <c r="C6" s="1">
         <v>1.72983E-5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="4">
+        <v>-1.25</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>3000</v>
       </c>
@@ -423,8 +496,16 @@
       <c r="C7" s="1">
         <v>1.7131099999999999E-5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="4">
+        <v>-4.5</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>3500</v>
       </c>
@@ -434,8 +515,16 @@
       <c r="C8" s="1">
         <v>1.6963E-5</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="4">
+        <v>-7.75</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>4000</v>
       </c>
@@ -445,8 +534,16 @@
       <c r="C9" s="1">
         <v>1.6793999999999999E-5</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="4">
+        <v>-11</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>4500</v>
       </c>
@@ -456,8 +553,16 @@
       <c r="C10" s="1">
         <v>1.6624099999999999E-5</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="4">
+        <v>-14.25</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>5000</v>
       </c>
@@ -467,8 +572,16 @@
       <c r="C11" s="1">
         <v>1.64531E-5</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="4">
+        <v>-17.5</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>5500</v>
       </c>
@@ -478,8 +591,16 @@
       <c r="C12" s="1">
         <v>1.6281299999999999E-5</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="4">
+        <v>-20.75</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>6000</v>
       </c>
@@ -489,8 +610,16 @@
       <c r="C13" s="1">
         <v>1.61084E-5</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="4">
+        <v>-24</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>6500</v>
       </c>
@@ -500,8 +629,16 @@
       <c r="C14" s="1">
         <v>1.5934500000000001E-5</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="4">
+        <v>-27.25</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>7000</v>
       </c>
@@ -511,8 +648,16 @@
       <c r="C15" s="1">
         <v>1.5759600000000001E-5</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="4">
+        <v>-30.5</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>7500</v>
       </c>
@@ -522,8 +667,16 @@
       <c r="C16" s="1">
         <v>1.5583700000000001E-5</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="4">
+        <v>-33.75</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>8000</v>
       </c>
@@ -533,8 +686,16 @@
       <c r="C17" s="1">
         <v>1.54068E-5</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="4">
+        <v>-37</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>8500</v>
       </c>
@@ -544,8 +705,16 @@
       <c r="C18" s="1">
         <v>1.5228800000000001E-5</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="4">
+        <v>-40.25</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>9000</v>
       </c>
@@ -555,8 +724,16 @@
       <c r="C19" s="1">
         <v>1.5049799999999999E-5</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="4">
+        <v>-43.5</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>9500</v>
       </c>
@@ -566,8 +743,16 @@
       <c r="C20" s="1">
         <v>1.4869600000000001E-5</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="4">
+        <v>-46.75</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>10000</v>
       </c>
@@ -577,8 +762,16 @@
       <c r="C21" s="1">
         <v>1.46884E-5</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="4">
+        <v>-50</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>10500</v>
       </c>
@@ -588,8 +781,16 @@
       <c r="C22" s="1">
         <v>1.45061E-5</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="4">
+        <v>-53.25</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>11000</v>
       </c>
@@ -599,8 +800,16 @@
       <c r="C23" s="1">
         <v>1.4322600000000001E-5</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="4">
+        <v>-56.5</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>11500</v>
       </c>
@@ -610,8 +819,16 @@
       <c r="C24" s="1">
         <v>1.4322600000000001E-5</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="4">
+        <v>-56.5</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>12000</v>
       </c>
@@ -621,8 +838,16 @@
       <c r="C25" s="1">
         <v>1.4322600000000001E-5</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="4">
+        <v>-56.5</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>12500</v>
       </c>
@@ -632,8 +857,16 @@
       <c r="C26" s="1">
         <v>1.4322600000000001E-5</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="4">
+        <v>-56.5</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>13000</v>
       </c>
@@ -643,8 +876,16 @@
       <c r="C27" s="1">
         <v>1.4322600000000001E-5</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="4">
+        <v>-56.5</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>13500</v>
       </c>
@@ -654,8 +895,16 @@
       <c r="C28" s="1">
         <v>1.4322600000000001E-5</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="4">
+        <v>-56.5</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>14000</v>
       </c>
@@ -665,8 +914,16 @@
       <c r="C29" s="1">
         <v>1.4322600000000001E-5</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="4">
+        <v>-56.5</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>14500</v>
       </c>
@@ -676,8 +933,16 @@
       <c r="C30" s="1">
         <v>1.4322600000000001E-5</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="4">
+        <v>-56.5</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>15000</v>
       </c>
@@ -687,8 +952,16 @@
       <c r="C31" s="1">
         <v>1.4322600000000001E-5</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="4">
+        <v>-56.5</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>15500</v>
       </c>
@@ -698,8 +971,16 @@
       <c r="C32" s="1">
         <v>1.4322600000000001E-5</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="4">
+        <v>-56.5</v>
+      </c>
+      <c r="F32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>16000</v>
       </c>
@@ -709,8 +990,16 @@
       <c r="C33" s="1">
         <v>1.4322600000000001E-5</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="4">
+        <v>-56.5</v>
+      </c>
+      <c r="F33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>16500</v>
       </c>
@@ -720,8 +1009,16 @@
       <c r="C34" s="1">
         <v>1.4322600000000001E-5</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="4">
+        <v>-56.5</v>
+      </c>
+      <c r="F34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>17000</v>
       </c>
@@ -731,8 +1028,16 @@
       <c r="C35" s="1">
         <v>1.4322600000000001E-5</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" s="4">
+        <v>-56.5</v>
+      </c>
+      <c r="F35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>17500</v>
       </c>
@@ -742,8 +1047,16 @@
       <c r="C36" s="1">
         <v>1.4322600000000001E-5</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="4">
+        <v>-56.5</v>
+      </c>
+      <c r="F36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>18000</v>
       </c>
@@ -753,8 +1066,16 @@
       <c r="C37" s="1">
         <v>1.4322600000000001E-5</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" s="4">
+        <v>-56.5</v>
+      </c>
+      <c r="F37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>18500</v>
       </c>
@@ -764,8 +1085,16 @@
       <c r="C38" s="1">
         <v>1.4322600000000001E-5</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" s="4">
+        <v>-56.5</v>
+      </c>
+      <c r="F38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>19000</v>
       </c>
@@ -775,8 +1104,16 @@
       <c r="C39" s="1">
         <v>1.4322600000000001E-5</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" s="4">
+        <v>-56.5</v>
+      </c>
+      <c r="F39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+    </row>
+    <row r="40" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>19500</v>
       </c>
@@ -786,8 +1123,16 @@
       <c r="C40" s="1">
         <v>1.4322600000000001E-5</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" s="4">
+        <v>-56.5</v>
+      </c>
+      <c r="F40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+    </row>
+    <row r="41" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>20000</v>
       </c>
@@ -797,8 +1142,16 @@
       <c r="C41" s="1">
         <v>1.4322600000000001E-5</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" s="4">
+        <v>-56.5</v>
+      </c>
+      <c r="F41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+    </row>
+    <row r="42" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>20500</v>
       </c>
@@ -808,8 +1161,16 @@
       <c r="C42" s="1">
         <v>1.43509E-5</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" s="4">
+        <v>-56</v>
+      </c>
+      <c r="F42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+    </row>
+    <row r="43" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>21000</v>
       </c>
@@ -819,8 +1180,16 @@
       <c r="C43" s="1">
         <v>1.4379199999999999E-5</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" s="4">
+        <v>-55.5</v>
+      </c>
+      <c r="F43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+    </row>
+    <row r="44" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>21500</v>
       </c>
@@ -830,8 +1199,16 @@
       <c r="C44" s="1">
         <v>1.44074E-5</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" s="4">
+        <v>-55</v>
+      </c>
+      <c r="F44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+    </row>
+    <row r="45" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>22000</v>
       </c>
@@ -841,8 +1218,16 @@
       <c r="C45" s="1">
         <v>1.44357E-5</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" s="4">
+        <v>-54.5</v>
+      </c>
+      <c r="F45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+    </row>
+    <row r="46" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>22500</v>
       </c>
@@ -852,8 +1237,16 @@
       <c r="C46" s="1">
         <v>1.4463900000000001E-5</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" s="4">
+        <v>-54</v>
+      </c>
+      <c r="F46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+    </row>
+    <row r="47" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>23000</v>
       </c>
@@ -863,8 +1256,16 @@
       <c r="C47" s="1">
         <v>1.4491999999999999E-5</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" s="4">
+        <v>-53.5</v>
+      </c>
+      <c r="F47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+    </row>
+    <row r="48" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>23500</v>
       </c>
@@ -874,8 +1275,16 @@
       <c r="C48" s="1">
         <v>1.45202E-5</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" s="4">
+        <v>-53</v>
+      </c>
+      <c r="F48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+    </row>
+    <row r="49" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>24000</v>
       </c>
@@ -885,8 +1294,16 @@
       <c r="C49" s="1">
         <v>1.4548299999999999E-5</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" s="4">
+        <v>-52.5</v>
+      </c>
+      <c r="F49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+    </row>
+    <row r="50" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>24500</v>
       </c>
@@ -896,8 +1313,16 @@
       <c r="C50" s="1">
         <v>1.45763E-5</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" s="4">
+        <v>-52</v>
+      </c>
+      <c r="F50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+    </row>
+    <row r="51" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>25000</v>
       </c>
@@ -907,8 +1332,16 @@
       <c r="C51" s="1">
         <v>1.46044E-5</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" s="4">
+        <v>-51.5</v>
+      </c>
+      <c r="F51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+    </row>
+    <row r="52" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>25500</v>
       </c>
@@ -918,8 +1351,16 @@
       <c r="C52" s="1">
         <v>1.4632400000000001E-5</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" s="4">
+        <v>-51</v>
+      </c>
+      <c r="F52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+    </row>
+    <row r="53" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>26000</v>
       </c>
@@ -929,8 +1370,16 @@
       <c r="C53" s="1">
         <v>1.4660399999999999E-5</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" s="4">
+        <v>-50.5</v>
+      </c>
+      <c r="F53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+    </row>
+    <row r="54" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>26500</v>
       </c>
@@ -940,8 +1389,16 @@
       <c r="C54" s="1">
         <v>1.46884E-5</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" s="4">
+        <v>-50</v>
+      </c>
+      <c r="F54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+    </row>
+    <row r="55" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>27000</v>
       </c>
@@ -951,8 +1408,16 @@
       <c r="C55" s="1">
         <v>1.47164E-5</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" s="4">
+        <v>-49.5</v>
+      </c>
+      <c r="F55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+    </row>
+    <row r="56" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>27500</v>
       </c>
@@ -962,8 +1427,16 @@
       <c r="C56" s="1">
         <v>1.47443E-5</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" s="4">
+        <v>-49</v>
+      </c>
+      <c r="F56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+    </row>
+    <row r="57" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>28000</v>
       </c>
@@ -973,8 +1446,16 @@
       <c r="C57" s="1">
         <v>1.4772200000000001E-5</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" s="4">
+        <v>-48.5</v>
+      </c>
+      <c r="F57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+    </row>
+    <row r="58" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>28500</v>
       </c>
@@ -984,8 +1465,16 @@
       <c r="C58" s="1">
         <v>1.4800100000000001E-5</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" s="4">
+        <v>-48</v>
+      </c>
+      <c r="F58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+    </row>
+    <row r="59" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>29000</v>
       </c>
@@ -995,8 +1484,16 @@
       <c r="C59" s="1">
         <v>1.4827900000000001E-5</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" s="4">
+        <v>-47.5</v>
+      </c>
+      <c r="F59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+    </row>
+    <row r="60" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>29500</v>
       </c>
@@ -1006,8 +1503,16 @@
       <c r="C60" s="1">
         <v>1.4855700000000001E-5</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" s="4">
+        <v>-47</v>
+      </c>
+      <c r="F60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+    </row>
+    <row r="61" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>30000</v>
       </c>
@@ -1017,8 +1522,17 @@
       <c r="C61" s="1">
         <v>1.4883500000000001E-5</v>
       </c>
+      <c r="D61" s="4">
+        <v>-46.5</v>
+      </c>
+      <c r="F61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>